<commit_message>
issue #36: Batch submission of SRA projects.
</commit_message>
<xml_diff>
--- a/edge_ui/data/BatchExcelExample.xlsx
+++ b/edge_ui/data/BatchExcelExample.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chien-chi/Projects/edge-git/edge_ui/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chien-chi/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8DA0BA-B3D7-234D-AC11-F91762314484}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A1C9A3-061F-134E-9321-4BE412AB4C0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="2460" windowWidth="18740" windowHeight="9520" tabRatio="987" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26280" yWindow="8740" windowWidth="24080" windowHeight="11820" tabRatio="987" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -91,12 +91,78 @@
         </r>
       </text>
     </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{BC6AA9A2-523D-224F-99FA-F9DDCF8A4E8D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chienchi Lo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Single End Reads</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{596B7F0A-AA88-2A4D-8A7B-6EBD1D5C9B9C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chienchi Lo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Input SRA accession</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Project</t>
   </si>
@@ -110,37 +176,34 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Project 1</t>
-  </si>
-  <si>
     <t>PublicData/testData/Ecoli_10x.1.fastq</t>
   </si>
   <si>
     <t>PublicData/testData/Ecoli_10x.2.fastq</t>
   </si>
   <si>
-    <t>test batch input project 1</t>
-  </si>
-  <si>
-    <t>Project 2</t>
-  </si>
-  <si>
-    <t>test batch input project 2</t>
-  </si>
-  <si>
-    <t>Project 3</t>
-  </si>
-  <si>
-    <t>test batch input project 3</t>
-  </si>
-  <si>
-    <t>Project 4</t>
-  </si>
-  <si>
-    <t>test batch input project 4</t>
-  </si>
-  <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>SRA</t>
+  </si>
+  <si>
+    <t>SRR11241255</t>
+  </si>
+  <si>
+    <t>test batch with SRA accession</t>
+  </si>
+  <si>
+    <t>Project SE</t>
+  </si>
+  <si>
+    <t>test batch with SE input</t>
+  </si>
+  <si>
+    <t>test batch with PE project</t>
+  </si>
+  <si>
+    <t>Project PE</t>
   </si>
 </sst>
 </file>
@@ -511,23 +574,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.5"/>
     <col min="3" max="3" width="34.83203125"/>
     <col min="4" max="4" width="31.6640625" customWidth="1"/>
-    <col min="5" max="5" width="22"/>
-    <col min="6" max="1026" width="11.5"/>
+    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="1027" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,80 +602,64 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
+      <c r="E2" s="1"/>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
require unique for project name for batch submit
</commit_message>
<xml_diff>
--- a/edge_ui/data/BatchExcelExample.xlsx
+++ b/edge_ui/data/BatchExcelExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chien-chi/Projects/LANL_git/EDGE/edge_ui/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C206CBA-57DC-0640-B54A-82B2288905B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAF88A3-073F-8744-BA32-C62A364EBE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="900" windowWidth="41060" windowHeight="27900" tabRatio="987" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26680" yWindow="900" windowWidth="27920" windowHeight="27900" tabRatio="987" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -272,9 +272,6 @@
     <t>sra-title</t>
   </si>
   <si>
-    <t>Name of the project in EC19</t>
-  </si>
-  <si>
     <t>Paired-end forward Fastq</t>
   </si>
   <si>
@@ -1149,6 +1146,9 @@
   </si>
   <si>
     <t>PublicData/testData/SARS-COVID-test-swift-v2.2.fastq</t>
+  </si>
+  <si>
+    <t>Name of the project in EC19. Should be unique in this Batch submit</t>
   </si>
 </sst>
 </file>
@@ -1978,8 +1978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD1908"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2035,7 +2035,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>12</v>
@@ -2112,10 +2112,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>343</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>344</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H2" s="23" t="s">
         <v>46</v>
@@ -2135,7 +2135,7 @@
         <v>43928</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L2" s="23" t="s">
         <v>49</v>
@@ -2180,7 +2180,7 @@
         <v>34</v>
       </c>
       <c r="Z2" s="23" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AA2" s="23" t="s">
         <v>35</v>
@@ -2202,17 +2202,17 @@
       <c r="B3" s="23"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="23" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I3" s="23" t="s">
         <v>20</v>
@@ -2221,13 +2221,13 @@
         <v>44235</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L3" s="23" t="s">
         <v>49</v>
       </c>
       <c r="M3" s="23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="N3" s="23">
         <v>33</v>
@@ -2236,28 +2236,28 @@
         <v>21</v>
       </c>
       <c r="P3" s="23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Q3" s="23" t="s">
         <v>47</v>
       </c>
       <c r="R3" s="23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S3" s="23" t="s">
         <v>21</v>
       </c>
       <c r="T3" s="23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="U3" s="23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="V3" s="23" t="s">
+        <v>320</v>
+      </c>
+      <c r="W3" s="23" t="s">
         <v>321</v>
-      </c>
-      <c r="W3" s="23" t="s">
-        <v>322</v>
       </c>
       <c r="X3" s="23" t="s">
         <v>33</v>
@@ -2266,7 +2266,7 @@
         <v>34</v>
       </c>
       <c r="Z3" s="23" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AA3" s="23" t="s">
         <v>35</v>
@@ -2278,7 +2278,7 @@
         <v>37</v>
       </c>
       <c r="AD3" s="23" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="15" x14ac:dyDescent="0.2">
@@ -2295,10 +2295,10 @@
         <v>7</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I4" s="23" t="s">
         <v>20</v>
@@ -2307,13 +2307,13 @@
         <v>44235</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L4" s="23" t="s">
         <v>49</v>
       </c>
       <c r="M4" s="23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="N4" s="23">
         <v>74</v>
@@ -2322,28 +2322,28 @@
         <v>21</v>
       </c>
       <c r="P4" s="23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Q4" s="23" t="s">
         <v>47</v>
       </c>
       <c r="R4" s="23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="S4" s="23" t="s">
         <v>21</v>
       </c>
       <c r="T4" s="23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="U4" s="23" t="s">
+        <v>319</v>
+      </c>
+      <c r="V4" s="23" t="s">
         <v>320</v>
       </c>
-      <c r="V4" s="23" t="s">
+      <c r="W4" s="23" t="s">
         <v>321</v>
-      </c>
-      <c r="W4" s="23" t="s">
-        <v>322</v>
       </c>
       <c r="X4" s="23" t="s">
         <v>33</v>
@@ -2352,7 +2352,7 @@
         <v>34</v>
       </c>
       <c r="Z4" s="23" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AA4" s="23" t="s">
         <v>35</v>
@@ -2364,7 +2364,7 @@
         <v>37</v>
       </c>
       <c r="AD4" s="23" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.15">
@@ -8140,8 +8140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{782CEA89-FD01-D74B-B501-1A22DC7A4236}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8154,7 +8154,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="77" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -8162,7 +8162,7 @@
     </row>
     <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -8170,7 +8170,7 @@
     </row>
     <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -8178,7 +8178,7 @@
     </row>
     <row r="4" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -8186,7 +8186,7 @@
     </row>
     <row r="5" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -8194,7 +8194,7 @@
     </row>
     <row r="6" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -8202,7 +8202,7 @@
     </row>
     <row r="7" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -8210,7 +8210,7 @@
     </row>
     <row r="8" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -8218,7 +8218,7 @@
     </row>
     <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -8226,7 +8226,7 @@
     </row>
     <row r="10" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -8234,7 +8234,7 @@
     </row>
     <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -8242,7 +8242,7 @@
     </row>
     <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -8260,24 +8260,24 @@
     <row r="15" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="43"/>
       <c r="B15" s="43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="40" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>52</v>
+        <v>344</v>
       </c>
       <c r="D16" s="42" t="s">
         <v>45</v>
@@ -8289,10 +8289,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8301,10 +8301,10 @@
         <v>2</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8313,7 +8313,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="19"/>
     </row>
@@ -8323,7 +8323,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="19"/>
     </row>
@@ -8333,24 +8333,24 @@
         <v>3</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="19" t="s">
         <v>62</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -8359,7 +8359,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>46</v>
@@ -8371,7 +8371,7 @@
         <v>40</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>20</v>
@@ -8383,10 +8383,10 @@
         <v>13</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -8395,10 +8395,10 @@
         <v>14</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -8407,7 +8407,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>49</v>
@@ -8419,7 +8419,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>21</v>
@@ -8431,7 +8431,7 @@
         <v>17</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>21</v>
@@ -8443,7 +8443,7 @@
         <v>18</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>21</v>
@@ -8455,7 +8455,7 @@
         <v>19</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>22</v>
@@ -8467,7 +8467,7 @@
         <v>39</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>47</v>
@@ -8479,7 +8479,7 @@
         <v>41</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>48</v>
@@ -8491,7 +8491,7 @@
         <v>42</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>21</v>
@@ -8503,10 +8503,10 @@
         <v>43</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8515,7 +8515,7 @@
         <v>44</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>50</v>
@@ -8523,13 +8523,13 @@
     </row>
     <row r="37" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>51</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>31</v>
@@ -8541,7 +8541,7 @@
         <v>23</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>32</v>
@@ -8553,7 +8553,7 @@
         <v>24</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>33</v>
@@ -8565,7 +8565,7 @@
         <v>25</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>34</v>
@@ -8577,10 +8577,10 @@
         <v>26</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -8589,7 +8589,7 @@
         <v>27</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D42" s="19" t="s">
         <v>35</v>
@@ -8601,7 +8601,7 @@
         <v>28</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D43" s="19" t="s">
         <v>36</v>
@@ -8613,7 +8613,7 @@
         <v>29</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D44" s="19" t="s">
         <v>37</v>
@@ -8625,10 +8625,10 @@
         <v>30</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -8671,7 +8671,7 @@
     </row>
     <row r="2" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B2" s="54"/>
       <c r="C2" s="55"/>
@@ -8684,73 +8684,73 @@
     </row>
     <row r="3" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="28" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C3" s="52"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C4" s="52"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="28" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C5" s="52"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C6" s="52"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="28" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C7" s="52"/>
     </row>
     <row r="8" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C8" s="52"/>
     </row>
     <row r="9" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="28" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C9" s="52"/>
     </row>
     <row r="10" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C10" s="52"/>
     </row>
@@ -8759,97 +8759,97 @@
         <v>34</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C11" s="52"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C12" s="52"/>
     </row>
     <row r="13" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C13" s="52"/>
     </row>
     <row r="14" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="28" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C14" s="52"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C15" s="52"/>
     </row>
     <row r="16" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="28" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C16" s="52"/>
     </row>
     <row r="17" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C17" s="52"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C18" s="52"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="28" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B19" s="52" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C19" s="52"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="28" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C20" s="52"/>
     </row>
     <row r="21" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B21" s="52" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C21" s="52"/>
       <c r="D21" s="26"/>
@@ -8861,135 +8861,135 @@
     </row>
     <row r="22" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B22" s="52" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C22" s="52"/>
     </row>
     <row r="23" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="28" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C23" s="52"/>
     </row>
     <row r="24" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B24" s="52" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C24" s="52"/>
     </row>
     <row r="25" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C26" s="26"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="26" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C27" s="26"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C28" s="26"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="26" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C29" s="26"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C30" s="26"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="26" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C32" s="26"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C33" s="26"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C34" s="26"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="26"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="26"/>
     </row>
     <row r="37" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B37" s="52" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C37" s="52"/>
     </row>
@@ -8999,53 +8999,53 @@
     </row>
     <row r="39" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B39" s="54"/>
       <c r="C39" s="55"/>
     </row>
     <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B40" s="52" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C40" s="52"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B41" s="52" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="26" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B42" s="52" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C42" s="52"/>
     </row>
     <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B43" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C43" s="52"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" s="26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B44" s="52" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C44" s="52"/>
     </row>
@@ -9060,20 +9060,20 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="26" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="26" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="26" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B48" s="52" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C48" s="52"/>
     </row>
@@ -9083,17 +9083,17 @@
     </row>
     <row r="50" spans="1:3" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B50" s="53"/>
       <c r="C50" s="52"/>
     </row>
     <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B51" s="52" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C51" s="52"/>
     </row>
@@ -9102,277 +9102,277 @@
         <v>33</v>
       </c>
       <c r="B52" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C52" s="52"/>
     </row>
     <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B53" s="52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C53" s="52"/>
     </row>
     <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B54" s="52" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C54" s="52"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B55" s="52" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C55" s="52"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B56" s="52" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C56" s="52"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B57" s="52" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C57" s="52"/>
     </row>
     <row r="58" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B58" s="52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C58" s="52"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B59" s="52" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C59" s="52"/>
     </row>
     <row r="60" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B60" s="52" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C60" s="52"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B61" s="52" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C61" s="52"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B62" s="52" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C62" s="52"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B63" s="52" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C63" s="52"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B64" s="52" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C64" s="52"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B65" s="52" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C65" s="52"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A66" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B66" s="52" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C66" s="52"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B67" s="52" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C67" s="52"/>
     </row>
     <row r="68" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B68" s="52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C68" s="52"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A69" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B69" s="52" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C69" s="52"/>
     </row>
     <row r="70" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B70" s="52" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C70" s="52"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A71" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B71" s="52" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C71" s="52"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B72" s="52" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C72" s="52"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A73" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B73" s="52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C73" s="52"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" s="28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B74" s="52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C74" s="52"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A75" s="28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B75" s="52" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C75" s="52"/>
     </row>
     <row r="76" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B76" s="52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C76" s="52"/>
     </row>
     <row r="77" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B77" s="52" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C77" s="52"/>
     </row>
     <row r="78" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B78" s="26"/>
     </row>
     <row r="79" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B79" s="26"/>
     </row>
     <row r="80" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A83" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
@@ -9381,178 +9381,178 @@
     </row>
     <row r="85" spans="1:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A85" s="36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="86" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A86" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B86" s="35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C86" s="34" t="s">
         <v>36</v>
       </c>
       <c r="D86" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E86" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F86" s="33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G86" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H86" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I86" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J86" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K86" s="33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A87" s="31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B87" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C87" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D87" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E87" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F87" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G87" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H87" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I87" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J87" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K87" s="26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="16" x14ac:dyDescent="0.15">
       <c r="A88" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B88" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C88" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E88" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G88" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H88" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I88" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J88" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K88" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="16" x14ac:dyDescent="0.15">
       <c r="A89" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B89" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C89" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E89" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G89" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H89" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I89" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J89" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K89" s="32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="16" x14ac:dyDescent="0.15">
       <c r="A90" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B90" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C90" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E90" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G90" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H90" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I90" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K90" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="28" x14ac:dyDescent="0.15">
       <c r="A91" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B91" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C91" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E91" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I91" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="14" x14ac:dyDescent="0.15">
@@ -9560,85 +9560,85 @@
         <v>36</v>
       </c>
       <c r="B92" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C92" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E92" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I92" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A93" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C93" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E93" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I93" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A94" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C94" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E94" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C95" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E95" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="C96" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E96" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="C97" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="C98" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="C99" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C100" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C101" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -9648,89 +9648,89 @@
     </row>
     <row r="103" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="C103" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="C104" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A107" s="37" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B107" s="37"/>
       <c r="C107" s="37" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A108" s="38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B108" s="38"/>
       <c r="C108" s="38" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A109" s="38" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B109" s="38"/>
       <c r="C109" s="38" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A110" s="38" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B110" s="38"/>
       <c r="C110" s="38" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A111" s="38" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B111" s="38"/>
       <c r="C111" s="38" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A112" s="38" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B112" s="38"/>
       <c r="C112" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A113" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B113" s="38"/>
       <c r="C113" s="38" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A114" s="38" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B114" s="38"/>
       <c r="C114" s="38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A115" s="38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B115" s="38"/>
       <c r="C115" s="38" t="s">
@@ -9743,12 +9743,12 @@
       </c>
       <c r="B116" s="26"/>
       <c r="C116" s="38" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A117" s="38" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B117" s="26"/>
       <c r="C117" s="26"/>

</xml_diff>

<commit_message>
support contigs fasta batch submit
</commit_message>
<xml_diff>
--- a/edge_ui/data/BatchExcelExample.xlsx
+++ b/edge_ui/data/BatchExcelExample.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chien-chi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chien-chi/Projects/edge-git/edge_ui/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A1C9A3-061F-134E-9321-4BE412AB4C0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9847BB8C-3CFC-B748-AD77-1A1A56EEC13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26280" yWindow="8740" windowWidth="24080" windowHeight="11820" tabRatio="987" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -157,12 +157,45 @@
         </r>
       </text>
     </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{0828F686-EE6D-964E-802A-39A939DA8196}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chienchi Lo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Contig FASTA inpput</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Project</t>
   </si>
@@ -204,6 +237,18 @@
   </si>
   <si>
     <t>Project PE</t>
+  </si>
+  <si>
+    <t>Contigs</t>
+  </si>
+  <si>
+    <t>test batch with contigs FASTA</t>
+  </si>
+  <si>
+    <t>PublicData/testData/contigs.fa</t>
+  </si>
+  <si>
+    <t>Project Contig</t>
   </si>
 </sst>
 </file>
@@ -256,10 +301,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,24 +618,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="34.5"/>
     <col min="3" max="3" width="34.83203125"/>
     <col min="4" max="4" width="31.6640625" customWidth="1"/>
     <col min="5" max="5" width="22.1640625" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="1027" width="11.5"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="1028" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,11 +652,14 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -623,11 +671,12 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -636,11 +685,12 @@
         <v>4</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1"/>
+      <c r="G3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -650,16 +700,25 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1"/>
+      <c r="G4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>